<commit_message>
Arregladas fechas y agregado un .exe
</commit_message>
<xml_diff>
--- a/datosTrabajadores.xlsx
+++ b/datosTrabajadores.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ci</t>
   </si>
@@ -73,13 +73,19 @@
   </si>
   <si>
     <t>developer</t>
+  </si>
+  <si>
+    <t>09/08/1997</t>
+  </si>
+  <si>
+    <t>01/08/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +95,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -233,7 +247,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -254,7 +268,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,7 +575,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,8 +651,8 @@
       <c r="C3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="14">
-        <v>35651</v>
+      <c r="D3" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="E3" s="7">
         <v>221145</v>
@@ -647,8 +663,8 @@
       <c r="G3" s="8">
         <v>0.08</v>
       </c>
-      <c r="H3" s="14">
-        <v>44409</v>
+      <c r="H3" s="14" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -665,81 +681,81 @@
       <c r="A5" s="6"/>
       <c r="B5" s="12"/>
       <c r="C5" s="7"/>
-      <c r="D5" s="12"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="7"/>
       <c r="F5" s="12"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="12"/>
+      <c r="H5" s="14"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="12"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="7"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="7"/>
-      <c r="H6" s="12"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="12"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="12"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="7"/>
       <c r="F7" s="12"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="12"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
       <c r="B8" s="12"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="12"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="7"/>
       <c r="F8" s="12"/>
       <c r="G8" s="7"/>
-      <c r="H8" s="12"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="12"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="12"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="7"/>
       <c r="F9" s="12"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="12"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="12"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="12"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="7"/>
       <c r="F10" s="12"/>
       <c r="G10" s="7"/>
-      <c r="H10" s="12"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
       <c r="B11" s="12"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="12"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="7"/>
       <c r="F11" s="12"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="12"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
       <c r="B12" s="13"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="13"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="10"/>
       <c r="F12" s="13"/>
       <c r="G12" s="10"/>
-      <c r="H12" s="13"/>
+      <c r="H12" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Usa imports en vez de require, corrige errores
</commit_message>
<xml_diff>
--- a/datosTrabajadores.xlsx
+++ b/datosTrabajadores.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5233088E-8E81-4D0F-B7F9-FB7D1B3226E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080A4FFF-0D9D-440F-82C4-1FCFEB60A40A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,6 +12,9 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="I0">Hoja1!$I$2</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -676,7 +679,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>